<commit_message>
refactor: se modifico tablas de excel y se agregaron steps en el feature
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DataPeruRail.xlsx
+++ b/src/main/resources/excel/DataPeruRail.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonnatan\Desktop\Automatizacion\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonnatan.espinoza\Documents\Automatizacion\perurail\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901F5B77-DBA8-47C1-848C-B776BA568F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DE4E0F-ADE0-4F36-99B6-7D1FB605A206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30000" yWindow="1605" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{D6FC13CF-84CB-4B18-B401-F373B6B0EDD3}"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="3" r:id="rId1"/>
-    <sheet name="tickets" sheetId="4" r:id="rId2"/>
-    <sheet name="data" sheetId="5" r:id="rId3"/>
+    <sheet name="cabin" sheetId="4" r:id="rId2"/>
+    <sheet name="user" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -108,7 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +120,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -146,12 +154,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -168,9 +177,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +217,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -314,7 +323,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,7 +465,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -470,7 +479,7 @@
       <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
@@ -512,15 +521,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1616FE-ED94-4E11-B7AC-2D133B3795B0}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -531,7 +540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -542,30 +551,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>5</v>
       </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -574,10 +599,10 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="5" max="7" width="15.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
fix: se soluciono problema al entrar a trains
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DataPeruRail.xlsx
+++ b/src/main/resources/excel/DataPeruRail.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonnatan.espinoza\Documents\Automatizacion\perurail\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B525B88-C498-43E8-A1C2-25090639C08B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822437E4-C98D-4BBF-8EEE-7F51B5832F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30000" yWindow="1605" windowWidth="21600" windowHeight="11295" xr2:uid="{D6FC13CF-84CB-4B18-B401-F373B6B0EDD3}"/>
+    <workbookView xWindow="30000" yWindow="1605" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{D6FC13CF-84CB-4B18-B401-F373B6B0EDD3}"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="3" r:id="rId1"/>
-    <sheet name="cabin" sheetId="4" r:id="rId2"/>
-    <sheet name="user" sheetId="5" r:id="rId3"/>
+    <sheet name="trains" sheetId="4" r:id="rId2"/>
+    <sheet name="passenger_data" sheetId="5" r:id="rId3"/>
+    <sheet name="confirmation_payment" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>tipo</t>
   </si>
@@ -53,15 +54,6 @@
     <t>SOLO IDA</t>
   </si>
   <si>
-    <t>cabina</t>
-  </si>
-  <si>
-    <t>adulto</t>
-  </si>
-  <si>
-    <t>ninho</t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
@@ -77,9 +69,6 @@
     <t>dni</t>
   </si>
   <si>
-    <t>cumpleanos</t>
-  </si>
-  <si>
     <t>telefono</t>
   </si>
   <si>
@@ -102,6 +91,129 @@
   </si>
   <si>
     <t>JOHN.DOE@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>tarjeta</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>MASTERCARD</t>
+  </si>
+  <si>
+    <t>AMERICAN</t>
+  </si>
+  <si>
+    <t>PAYPAL</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>TW</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>IDA Y VUELTA</t>
+  </si>
+  <si>
+    <t>PERURAIL EXPEDITION</t>
+  </si>
+  <si>
+    <t>AREQUIPA</t>
+  </si>
+  <si>
+    <t>MACHUPICCHU</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>cumpleanhos</t>
+  </si>
+  <si>
+    <t>JANE</t>
+  </si>
+  <si>
+    <t>SMITH</t>
+  </si>
+  <si>
+    <t>JANE.SMITH@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>cab1 ninho</t>
+  </si>
+  <si>
+    <t>cab2 ninho</t>
+  </si>
+  <si>
+    <t>cab3 ninho</t>
+  </si>
+  <si>
+    <t>cab4 ninho</t>
+  </si>
+  <si>
+    <t>cab5 ninho</t>
+  </si>
+  <si>
+    <t>cab7 ninho</t>
+  </si>
+  <si>
+    <t>cab8 ninho</t>
+  </si>
+  <si>
+    <t>JUAN</t>
+  </si>
+  <si>
+    <t>PEREZ</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>JUAN.PEREZ@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>cab1 adulto</t>
+  </si>
+  <si>
+    <t>cab2 adulto</t>
+  </si>
+  <si>
+    <t>cab3 adulto</t>
+  </si>
+  <si>
+    <t>cab4 adulto</t>
+  </si>
+  <si>
+    <t>cab5 adulto</t>
+  </si>
+  <si>
+    <t>cab6 adulto</t>
+  </si>
+  <si>
+    <t>cab6 ninho</t>
+  </si>
+  <si>
+    <t>cab7 adulto</t>
+  </si>
+  <si>
+    <t>cab8 adulto</t>
+  </si>
+  <si>
+    <t>ADULTO</t>
+  </si>
+  <si>
+    <t>NINHO</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -133,18 +245,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -154,16 +287,385 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="42">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="4"/>
+        </left>
+        <right style="medium">
+          <color theme="4"/>
+        </right>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="4"/>
+        </left>
+        <right style="medium">
+          <color theme="4"/>
+        </right>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="4"/>
+        </left>
+        <right style="medium">
+          <color theme="4"/>
+        </right>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="4"/>
+        </left>
+        <right style="medium">
+          <color theme="4"/>
+        </right>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -174,6 +676,118 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1652CAA9-7C57-4CC6-AF28-FF59B7024886}" name="Tabla3" displayName="Tabla3" ref="A1:E4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="16">
+  <autoFilter ref="A1:E4" xr:uid="{EC49B573-A6C0-438B-8D7D-6033A5C9240C}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{AF1F70C4-EEAF-46BC-B521-48F7B8178DC1}" name="id" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{8D365490-8F6C-4CB3-A978-A767CF110BD2}" name="tipo" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{407BDEB2-50A9-4547-BE98-80B3548B87E2}" name="servicio" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{2E7B4E0A-59DD-4509-84CC-121416A1D0EA}" name="partida" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{4C6E8BCC-4CD2-453E-908C-0E6BD877430C}" name="destino" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1342713E-B4EB-4B05-95AC-7413F77FCB87}" name="Tabla1" displayName="Tabla1" ref="A1:S4" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
+  <autoFilter ref="A1:S4" xr:uid="{9EAAADC5-9F46-43F9-86DA-9355898506F0}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
+    <filterColumn colId="17" hiddenButton="1"/>
+    <filterColumn colId="18" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{1B96264B-2CB3-47D7-B4C0-51870E444072}" name="Id" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{F471FA38-E69A-47DD-80E5-6DB2A13DA5F2}" name="tipo" dataDxfId="17"/>
+    <tableColumn id="27" xr3:uid="{593C92AB-FB00-425B-BAE4-125BCD359769}" name="n" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{2CB10096-B030-40AC-A185-5BAF05E5996A}" name="cab1 adulto" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{4BF48631-0A0C-4A8D-BDDC-A6363B600754}" name="cab1 ninho" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{782AF4A2-3991-40DA-87D7-CFBF36B6D3CF}" name="cab2 adulto" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{2D21EED6-3A13-4F76-B9EB-3D0CEDBA098A}" name="cab2 ninho" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{B3826654-211E-4333-8145-ED5B6A0713B3}" name="cab3 adulto" dataDxfId="30"/>
+    <tableColumn id="11" xr3:uid="{66740B94-F52D-4E67-9DE4-A6F7D5C1D86A}" name="cab3 ninho" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{ABC75B57-996C-499F-A86A-BEF43DA1822A}" name="cab4 adulto" dataDxfId="28"/>
+    <tableColumn id="14" xr3:uid="{742E54BC-8B8A-46CA-86E8-E57426D99AA0}" name="cab4 ninho" dataDxfId="27"/>
+    <tableColumn id="15" xr3:uid="{0C3C72A8-0EFF-4257-89CF-DA314D58045D}" name="cab5 adulto" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{1B1E8A8C-8FE2-4FB4-A0B3-D6B67CCE0051}" name="cab5 ninho" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{B3CE59D7-3C6F-493F-B16E-90E99B4687E8}" name="cab6 adulto" dataDxfId="24"/>
+    <tableColumn id="20" xr3:uid="{883376CA-564F-46C6-A8AA-1ABBCFB17391}" name="cab6 ninho" dataDxfId="23"/>
+    <tableColumn id="21" xr3:uid="{A554B50B-B826-42AE-BF9F-6322C26F7556}" name="cab7 adulto" dataDxfId="22"/>
+    <tableColumn id="23" xr3:uid="{E47090D1-C062-483F-8F35-AB1D2E620891}" name="cab7 ninho" dataDxfId="21"/>
+    <tableColumn id="24" xr3:uid="{67CFF31E-6EEB-436D-966A-F6924BE14906}" name="cab8 adulto" dataDxfId="20"/>
+    <tableColumn id="26" xr3:uid="{62CF0A50-024F-419D-A148-FE2CD3007DED}" name="cab8 ninho" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87305A22-35F9-42EC-9298-4EBF5F16E71E}" name="Tabla4" displayName="Tabla4" ref="A1:J4" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="10">
+  <autoFilter ref="A1:J4" xr:uid="{A59B09B4-BE40-4769-A458-C2BBB98E1FD2}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{A67B8055-A31F-4E61-B923-53E93F83D94D}" name="id" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{E4C9E876-2CE6-46DD-ABF6-BD84C1ABADE0}" name="tipo" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4EFD328A-F656-4EB3-BAF8-BBFE9DA54446}" name="nombre"/>
+    <tableColumn id="3" xr3:uid="{B64115F5-DB6E-4390-9D72-B28B899FBE63}" name="apellido"/>
+    <tableColumn id="4" xr3:uid="{371A0582-D500-48FA-9125-FE8C3A19B89D}" name="genero" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{553FB7E9-1C69-4B90-AF93-03D6DB9D2E9B}" name="pais" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{D44FC6FC-48E1-4D14-AA44-6EAC0ED03876}" name="dni" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{14698F99-1A4C-4D41-AD0C-1EE9DD2E71C6}" name="cumpleanhos" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{D44FF9C0-E498-4360-B1D1-2F753CE8B9E1}" name="telefono" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{68E432A6-4D1E-4442-8D04-4B3C3DD39AD1}" name="correo" dataCellStyle="Hipervínculo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{541625AD-5C97-4AD0-BBB7-D671FD0CF7AA}" name="Tabla2" displayName="Tabla2" ref="A1:B5" totalsRowShown="0" tableBorderDxfId="3">
+  <autoFilter ref="A1:B5" xr:uid="{5AF637C0-FB21-4C41-BD79-56E1E1BC8907}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="2" xr3:uid="{AF9C8BCC-2BEC-4484-BF1A-C0EE8806C782}" name="id" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3D223BA8-F0C0-4743-98A6-044389749B02}" name="tarjeta"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,198 +1087,582 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD712343-5B09-4611-8630-A5A24B98FDC8}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1616FE-ED94-4E11-B7AC-2D133B3795B0}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" style="3" customWidth="1"/>
+    <col min="6" max="13" width="9.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="9">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9">
+        <v>0</v>
+      </c>
+      <c r="I2" s="13">
+        <v>0</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0</v>
+      </c>
+      <c r="K2" s="13">
+        <v>0</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0</v>
+      </c>
+      <c r="M2" s="13">
+        <v>0</v>
+      </c>
+      <c r="N2" s="9">
+        <v>0</v>
+      </c>
+      <c r="O2" s="13">
+        <v>0</v>
+      </c>
+      <c r="P2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="13">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
+        <v>0</v>
+      </c>
+      <c r="S2" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="E3" s="13">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="2"/>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0</v>
+      </c>
+      <c r="K3" s="13">
+        <v>0</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0</v>
+      </c>
+      <c r="M3" s="13">
+        <v>0</v>
+      </c>
+      <c r="N3" s="9">
+        <v>0</v>
+      </c>
+      <c r="O3" s="13">
+        <v>0</v>
+      </c>
+      <c r="P3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="13">
+        <v>0</v>
+      </c>
+      <c r="R3" s="9">
+        <v>0</v>
+      </c>
+      <c r="S3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="13">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="9">
+        <v>0</v>
+      </c>
+      <c r="O4" s="13">
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>0</v>
+      </c>
+      <c r="R4" s="9">
+        <v>0</v>
+      </c>
+      <c r="S4" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7E65F2-5786-4038-91E1-AB94B5AD9FAC}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-    <col min="5" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="1" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="7" max="9" width="15.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="E2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="F2" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G2" s="6">
+        <v>10000001</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
+      <c r="I2" s="6">
+        <v>999888777</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2">
-        <v>12345678</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2">
-        <v>989697686</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>24</v>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="6">
+        <v>10000002</v>
+      </c>
+      <c r="H3" s="16">
+        <v>36695</v>
+      </c>
+      <c r="I3" s="6">
+        <v>999888778</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4">
+        <v>10000003</v>
+      </c>
+      <c r="H4" s="8">
+        <v>39617</v>
+      </c>
+      <c r="I4" s="4">
+        <v>999888779</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{EDBE7E2E-DF90-4605-BB0E-E8CF6B41AC41}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{EDBE7E2E-DF90-4605-BB0E-E8CF6B41AC41}"/>
+    <hyperlink ref="J3" r:id="rId2" xr:uid="{B2FCA654-2C91-46BB-9DAD-1788CF7E4EAD}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{E97F2C90-A4BB-4694-9B1B-52934912DD2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BDDB9-123C-42C7-8772-2B03ABCF962E}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: se completo el paso trenes
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DataPeruRail.xlsx
+++ b/src/main/resources/excel/DataPeruRail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonnatan.espinoza\Documents\Automatizacion\perurail\src\main\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonnatan\Desktop\Automatizacion\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822437E4-C98D-4BBF-8EEE-7F51B5832F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D10773-E0F6-42C9-83EC-FEC7059D870F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30000" yWindow="1605" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{D6FC13CF-84CB-4B18-B401-F373B6B0EDD3}"/>
+    <workbookView xWindow="795" yWindow="2025" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{D6FC13CF-84CB-4B18-B401-F373B6B0EDD3}"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
   <si>
     <t>tipo</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>CS</t>
-  </si>
-  <si>
     <t>TW</t>
   </si>
   <si>
@@ -214,6 +211,75 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PER </t>
+  </si>
+  <si>
+    <t>21/05/1999</t>
+  </si>
+  <si>
+    <t>15/09/2001</t>
+  </si>
+  <si>
+    <t>29/10/2000</t>
+  </si>
+  <si>
+    <t>MARIA.GONZALEZ@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>ROBERTO.FLORES@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>SOFIA.MARTINEZ@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>CARLOS.JIMENEZ@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>LUCIA.MORENO@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>DIEGO.SUAREZ@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>CARLOS</t>
+  </si>
+  <si>
+    <t>LUCIA</t>
+  </si>
+  <si>
+    <t>DIEGO</t>
+  </si>
+  <si>
+    <t>JIMENEZ</t>
+  </si>
+  <si>
+    <t>MORENO</t>
+  </si>
+  <si>
+    <t>SUAREZ</t>
+  </si>
+  <si>
+    <t>SOFIA</t>
+  </si>
+  <si>
+    <t>ROBERTO</t>
+  </si>
+  <si>
+    <t>MARIA</t>
+  </si>
+  <si>
+    <t>MARTINEZ</t>
+  </si>
+  <si>
+    <t>FLORES</t>
+  </si>
+  <si>
+    <t>GONZALEZ</t>
   </si>
 </sst>
 </file>
@@ -287,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -297,25 +363,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -324,25 +384,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="42">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -380,6 +429,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color theme="4"/>
@@ -396,51 +448,10 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color theme="4"/>
-        </left>
-        <right style="medium">
-          <color theme="4"/>
-        </right>
-        <top style="medium">
-          <color theme="4"/>
-        </top>
-        <bottom style="medium">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -598,6 +609,25 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -638,10 +668,35 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color theme="4"/>
+        </left>
+        <right style="medium">
+          <color theme="4"/>
+        </right>
+        <top style="medium">
+          <color theme="4"/>
+        </top>
+        <bottom style="medium">
+          <color theme="4"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -679,7 +734,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1652CAA9-7C57-4CC6-AF28-FF59B7024886}" name="Tabla3" displayName="Tabla3" ref="A1:E4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1652CAA9-7C57-4CC6-AF28-FF59B7024886}" name="Tabla3" displayName="Tabla3" ref="A1:E4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="A1:E4" xr:uid="{EC49B573-A6C0-438B-8D7D-6033A5C9240C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -688,18 +743,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AF1F70C4-EEAF-46BC-B521-48F7B8178DC1}" name="id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{8D365490-8F6C-4CB3-A978-A767CF110BD2}" name="tipo" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{407BDEB2-50A9-4547-BE98-80B3548B87E2}" name="servicio" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{2E7B4E0A-59DD-4509-84CC-121416A1D0EA}" name="partida" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{4C6E8BCC-4CD2-453E-908C-0E6BD877430C}" name="destino" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{AF1F70C4-EEAF-46BC-B521-48F7B8178DC1}" name="id" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{8D365490-8F6C-4CB3-A978-A767CF110BD2}" name="tipo" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{407BDEB2-50A9-4547-BE98-80B3548B87E2}" name="servicio" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{2E7B4E0A-59DD-4509-84CC-121416A1D0EA}" name="partida" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{4C6E8BCC-4CD2-453E-908C-0E6BD877430C}" name="destino" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1342713E-B4EB-4B05-95AC-7413F77FCB87}" name="Tabla1" displayName="Tabla1" ref="A1:S4" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1342713E-B4EB-4B05-95AC-7413F77FCB87}" name="Tabla1" displayName="Tabla1" ref="A1:S4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A1:S4" xr:uid="{9EAAADC5-9F46-43F9-86DA-9355898506F0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -722,33 +777,33 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{1B96264B-2CB3-47D7-B4C0-51870E444072}" name="Id" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{F471FA38-E69A-47DD-80E5-6DB2A13DA5F2}" name="tipo" dataDxfId="17"/>
-    <tableColumn id="27" xr3:uid="{593C92AB-FB00-425B-BAE4-125BCD359769}" name="n" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{2CB10096-B030-40AC-A185-5BAF05E5996A}" name="cab1 adulto" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{4BF48631-0A0C-4A8D-BDDC-A6363B600754}" name="cab1 ninho" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{782AF4A2-3991-40DA-87D7-CFBF36B6D3CF}" name="cab2 adulto" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{2D21EED6-3A13-4F76-B9EB-3D0CEDBA098A}" name="cab2 ninho" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{B3826654-211E-4333-8145-ED5B6A0713B3}" name="cab3 adulto" dataDxfId="30"/>
-    <tableColumn id="11" xr3:uid="{66740B94-F52D-4E67-9DE4-A6F7D5C1D86A}" name="cab3 ninho" dataDxfId="29"/>
-    <tableColumn id="12" xr3:uid="{ABC75B57-996C-499F-A86A-BEF43DA1822A}" name="cab4 adulto" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{742E54BC-8B8A-46CA-86E8-E57426D99AA0}" name="cab4 ninho" dataDxfId="27"/>
-    <tableColumn id="15" xr3:uid="{0C3C72A8-0EFF-4257-89CF-DA314D58045D}" name="cab5 adulto" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{1B1E8A8C-8FE2-4FB4-A0B3-D6B67CCE0051}" name="cab5 ninho" dataDxfId="25"/>
-    <tableColumn id="18" xr3:uid="{B3CE59D7-3C6F-493F-B16E-90E99B4687E8}" name="cab6 adulto" dataDxfId="24"/>
-    <tableColumn id="20" xr3:uid="{883376CA-564F-46C6-A8AA-1ABBCFB17391}" name="cab6 ninho" dataDxfId="23"/>
-    <tableColumn id="21" xr3:uid="{A554B50B-B826-42AE-BF9F-6322C26F7556}" name="cab7 adulto" dataDxfId="22"/>
-    <tableColumn id="23" xr3:uid="{E47090D1-C062-483F-8F35-AB1D2E620891}" name="cab7 ninho" dataDxfId="21"/>
-    <tableColumn id="24" xr3:uid="{67CFF31E-6EEB-436D-966A-F6924BE14906}" name="cab8 adulto" dataDxfId="20"/>
-    <tableColumn id="26" xr3:uid="{62CF0A50-024F-419D-A148-FE2CD3007DED}" name="cab8 ninho" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{1B96264B-2CB3-47D7-B4C0-51870E444072}" name="Id" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{F471FA38-E69A-47DD-80E5-6DB2A13DA5F2}" name="tipo" dataDxfId="29"/>
+    <tableColumn id="27" xr3:uid="{593C92AB-FB00-425B-BAE4-125BCD359769}" name="n" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{2CB10096-B030-40AC-A185-5BAF05E5996A}" name="cab1 adulto" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{4BF48631-0A0C-4A8D-BDDC-A6363B600754}" name="cab1 ninho" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{782AF4A2-3991-40DA-87D7-CFBF36B6D3CF}" name="cab2 adulto" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{2D21EED6-3A13-4F76-B9EB-3D0CEDBA098A}" name="cab2 ninho" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{B3826654-211E-4333-8145-ED5B6A0713B3}" name="cab3 adulto" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{66740B94-F52D-4E67-9DE4-A6F7D5C1D86A}" name="cab3 ninho" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{ABC75B57-996C-499F-A86A-BEF43DA1822A}" name="cab4 adulto" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{742E54BC-8B8A-46CA-86E8-E57426D99AA0}" name="cab4 ninho" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{0C3C72A8-0EFF-4257-89CF-DA314D58045D}" name="cab5 adulto" dataDxfId="19"/>
+    <tableColumn id="17" xr3:uid="{1B1E8A8C-8FE2-4FB4-A0B3-D6B67CCE0051}" name="cab5 ninho" dataDxfId="18"/>
+    <tableColumn id="18" xr3:uid="{B3CE59D7-3C6F-493F-B16E-90E99B4687E8}" name="cab6 adulto" dataDxfId="17"/>
+    <tableColumn id="20" xr3:uid="{883376CA-564F-46C6-A8AA-1ABBCFB17391}" name="cab6 ninho" dataDxfId="16"/>
+    <tableColumn id="21" xr3:uid="{A554B50B-B826-42AE-BF9F-6322C26F7556}" name="cab7 adulto" dataDxfId="15"/>
+    <tableColumn id="23" xr3:uid="{E47090D1-C062-483F-8F35-AB1D2E620891}" name="cab7 ninho" dataDxfId="14"/>
+    <tableColumn id="24" xr3:uid="{67CFF31E-6EEB-436D-966A-F6924BE14906}" name="cab8 adulto" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{62CF0A50-024F-419D-A148-FE2CD3007DED}" name="cab8 ninho" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87305A22-35F9-42EC-9298-4EBF5F16E71E}" name="Tabla4" displayName="Tabla4" ref="A1:J4" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" tableBorderDxfId="10">
-  <autoFilter ref="A1:J4" xr:uid="{A59B09B4-BE40-4769-A458-C2BBB98E1FD2}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87305A22-35F9-42EC-9298-4EBF5F16E71E}" name="Tabla4" displayName="Tabla4" ref="A1:J10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:J10" xr:uid="{A59B09B4-BE40-4769-A458-C2BBB98E1FD2}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -761,29 +816,29 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A67B8055-A31F-4E61-B923-53E93F83D94D}" name="id" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{E4C9E876-2CE6-46DD-ABF6-BD84C1ABADE0}" name="tipo" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A67B8055-A31F-4E61-B923-53E93F83D94D}" name="id" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{E4C9E876-2CE6-46DD-ABF6-BD84C1ABADE0}" name="tipo" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{4EFD328A-F656-4EB3-BAF8-BBFE9DA54446}" name="nombre"/>
     <tableColumn id="3" xr3:uid="{B64115F5-DB6E-4390-9D72-B28B899FBE63}" name="apellido"/>
-    <tableColumn id="4" xr3:uid="{371A0582-D500-48FA-9125-FE8C3A19B89D}" name="genero" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{553FB7E9-1C69-4B90-AF93-03D6DB9D2E9B}" name="pais" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{D44FC6FC-48E1-4D14-AA44-6EAC0ED03876}" name="dni" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{14698F99-1A4C-4D41-AD0C-1EE9DD2E71C6}" name="cumpleanhos" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{D44FF9C0-E498-4360-B1D1-2F753CE8B9E1}" name="telefono" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{68E432A6-4D1E-4442-8D04-4B3C3DD39AD1}" name="correo" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="4" xr3:uid="{371A0582-D500-48FA-9125-FE8C3A19B89D}" name="genero" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{553FB7E9-1C69-4B90-AF93-03D6DB9D2E9B}" name="pais" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{D44FC6FC-48E1-4D14-AA44-6EAC0ED03876}" name="dni" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{14698F99-1A4C-4D41-AD0C-1EE9DD2E71C6}" name="cumpleanhos" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{D44FF9C0-E498-4360-B1D1-2F753CE8B9E1}" name="telefono" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{68E432A6-4D1E-4442-8D04-4B3C3DD39AD1}" name="correo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{541625AD-5C97-4AD0-BBB7-D671FD0CF7AA}" name="Tabla2" displayName="Tabla2" ref="A1:B5" totalsRowShown="0" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{541625AD-5C97-4AD0-BBB7-D671FD0CF7AA}" name="Tabla2" displayName="Tabla2" ref="A1:B5" totalsRowShown="0" tableBorderDxfId="1">
   <autoFilter ref="A1:B5" xr:uid="{5AF637C0-FB21-4C41-BD79-56E1E1BC8907}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{AF9C8BCC-2BEC-4484-BF1A-C0EE8806C782}" name="id" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{AF9C8BCC-2BEC-4484-BF1A-C0EE8806C782}" name="id" dataDxfId="0"/>
     <tableColumn id="1" xr3:uid="{3D223BA8-F0C0-4743-98A6-044389749B02}" name="tarjeta"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -791,9 +846,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -831,7 +886,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -937,7 +992,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1079,7 +1134,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1093,7 +1148,7 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1102,71 +1157,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1182,10 +1237,10 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="5" width="9.7109375" style="3" customWidth="1"/>
@@ -1193,243 +1248,240 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="C2" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="E2" s="11">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>2</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0</v>
+      </c>
+      <c r="I2" s="11">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0</v>
+      </c>
+      <c r="M2" s="11">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="11">
+        <v>0</v>
+      </c>
+      <c r="R2" s="7">
+        <v>0</v>
+      </c>
+      <c r="S2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="F2" s="9">
-        <v>0</v>
-      </c>
-      <c r="G2" s="13">
-        <v>0</v>
-      </c>
-      <c r="H2" s="9">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13">
-        <v>0</v>
-      </c>
-      <c r="J2" s="9">
-        <v>0</v>
-      </c>
-      <c r="K2" s="13">
-        <v>0</v>
-      </c>
-      <c r="L2" s="9">
-        <v>0</v>
-      </c>
-      <c r="M2" s="13">
-        <v>0</v>
-      </c>
-      <c r="N2" s="9">
-        <v>0</v>
-      </c>
-      <c r="O2" s="13">
-        <v>0</v>
-      </c>
-      <c r="P2" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="13">
-        <v>0</v>
-      </c>
-      <c r="R2" s="9">
-        <v>0</v>
-      </c>
-      <c r="S2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="E3" s="11">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
+      <c r="K3" s="11">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="11">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+      <c r="O3" s="11">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>0</v>
+      </c>
+      <c r="R3" s="7">
+        <v>0</v>
+      </c>
+      <c r="S3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="13">
-        <v>1</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0</v>
-      </c>
-      <c r="G3" s="13">
-        <v>0</v>
-      </c>
-      <c r="H3" s="9">
-        <v>0</v>
-      </c>
-      <c r="I3" s="13">
-        <v>0</v>
-      </c>
-      <c r="J3" s="9">
-        <v>0</v>
-      </c>
-      <c r="K3" s="13">
-        <v>0</v>
-      </c>
-      <c r="L3" s="9">
-        <v>0</v>
-      </c>
-      <c r="M3" s="13">
-        <v>0</v>
-      </c>
-      <c r="N3" s="9">
-        <v>0</v>
-      </c>
-      <c r="O3" s="13">
-        <v>0</v>
-      </c>
-      <c r="P3" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="13">
-        <v>0</v>
-      </c>
-      <c r="R3" s="9">
-        <v>0</v>
-      </c>
-      <c r="S3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9">
-        <v>0</v>
-      </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="9">
-        <v>0</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9">
-        <v>0</v>
-      </c>
-      <c r="K4" s="13">
-        <v>0</v>
-      </c>
-      <c r="L4" s="9">
-        <v>0</v>
-      </c>
-      <c r="M4" s="13">
-        <v>0</v>
-      </c>
-      <c r="N4" s="9">
-        <v>0</v>
-      </c>
-      <c r="O4" s="13">
-        <v>0</v>
-      </c>
-      <c r="P4" s="9">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="13">
-        <v>0</v>
-      </c>
-      <c r="R4" s="9">
-        <v>0</v>
-      </c>
-      <c r="S4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="M6" s="17"/>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="11">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="11">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="M4" s="11">
+        <v>0</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0</v>
+      </c>
+      <c r="O4" s="11">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>0</v>
+      </c>
+      <c r="R4" s="7">
+        <v>0</v>
+      </c>
+      <c r="S4" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="I7" s="2"/>
@@ -1445,13 +1497,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7E65F2-5786-4038-91E1-AB94B5AD9FAC}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" customWidth="1"/>
@@ -1462,99 +1514,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4">
+        <v>10000001</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4">
+        <v>999888777</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6">
-        <v>10000001</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="6">
-        <v>999888777</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="G3" s="4">
+        <v>10000002</v>
+      </c>
+      <c r="H3" s="6">
+        <v>36695</v>
+      </c>
+      <c r="I3" s="4">
+        <v>999888778</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="6">
-        <v>10000002</v>
-      </c>
-      <c r="H3" s="16">
-        <v>36695</v>
-      </c>
-      <c r="I3" s="6">
-        <v>999888778</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1562,13 +1614,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
         <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>47</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>17</v>
@@ -1579,14 +1631,206 @@
       <c r="G4" s="4">
         <v>10000003</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="6">
         <v>39617</v>
       </c>
       <c r="I4" s="4">
         <v>999888779</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" s="4">
+        <v>10000004</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="4">
+        <v>999888780</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="4">
+        <v>10000005</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="4">
+        <v>999888781</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="4">
+        <v>10000006</v>
+      </c>
+      <c r="H7" s="6">
+        <v>40037</v>
+      </c>
+      <c r="I7" s="4">
+        <v>999888782</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="4">
+        <v>10000007</v>
+      </c>
+      <c r="H8" s="6">
+        <v>35861</v>
+      </c>
+      <c r="I8" s="4">
+        <v>999888783</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="4">
+        <v>10000008</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="4">
+        <v>999888784</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="4">
+        <v>10000009</v>
+      </c>
+      <c r="H10" s="6">
+        <v>40180</v>
+      </c>
+      <c r="I10" s="4">
+        <v>999888785</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1594,10 +1838,16 @@
     <hyperlink ref="J2" r:id="rId1" xr:uid="{EDBE7E2E-DF90-4605-BB0E-E8CF6B41AC41}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{B2FCA654-2C91-46BB-9DAD-1788CF7E4EAD}"/>
     <hyperlink ref="J4" r:id="rId3" xr:uid="{E97F2C90-A4BB-4694-9B1B-52934912DD2B}"/>
+    <hyperlink ref="J5" r:id="rId4" xr:uid="{DF9663D3-B01E-46EF-A09A-4DBE4CECECE5}"/>
+    <hyperlink ref="J6" r:id="rId5" xr:uid="{20E7BBE3-8014-4468-8C52-DEC6E4C6479A}"/>
+    <hyperlink ref="J7" r:id="rId6" xr:uid="{A797241E-92CF-4A97-AD88-E955311FBF43}"/>
+    <hyperlink ref="J8" r:id="rId7" xr:uid="{35CE8E0C-2660-4268-A92B-584BF595697F}"/>
+    <hyperlink ref="J9" r:id="rId8" xr:uid="{81B60F69-6326-42B7-85C0-B33B153BB8B3}"/>
+    <hyperlink ref="J10" r:id="rId9" xr:uid="{EEB17FD2-DDD6-4B99-A5ED-6EB9B1D56F90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1610,49 +1860,49 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: avance automatizacion flujo:passenger
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DataPeruRail.xlsx
+++ b/src/main/resources/excel/DataPeruRail.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhonnatan\Desktop\Automatizacion\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D10773-E0F6-42C9-83EC-FEC7059D870F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7372FD96-749E-4CA5-A60D-0580278B9509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="2025" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{D6FC13CF-84CB-4B18-B401-F373B6B0EDD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D6FC13CF-84CB-4B18-B401-F373B6B0EDD3}"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="3" r:id="rId1"/>
     <sheet name="trains" sheetId="4" r:id="rId2"/>
-    <sheet name="passenger_data" sheetId="5" r:id="rId3"/>
-    <sheet name="confirmation_payment" sheetId="6" r:id="rId4"/>
+    <sheet name="adult_data" sheetId="5" r:id="rId3"/>
+    <sheet name="children_data" sheetId="8" r:id="rId4"/>
+    <sheet name="confirmation_payment" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="126">
   <si>
     <t>tipo</t>
   </si>
@@ -174,9 +175,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>JUAN.PEREZ@GMAIL.COM</t>
-  </si>
-  <si>
     <t>cab1 adulto</t>
   </si>
   <si>
@@ -204,21 +202,12 @@
     <t>cab8 adulto</t>
   </si>
   <si>
-    <t>ADULTO</t>
-  </si>
-  <si>
-    <t>NINHO</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
     <t>SC</t>
   </si>
   <si>
-    <t xml:space="preserve">PER </t>
-  </si>
-  <si>
     <t>21/05/1999</t>
   </si>
   <si>
@@ -234,18 +223,12 @@
     <t>ROBERTO.FLORES@GMAIL.COM</t>
   </si>
   <si>
-    <t>SOFIA.MARTINEZ@GMAIL.COM</t>
-  </si>
-  <si>
     <t>CARLOS.JIMENEZ@GMAIL.COM</t>
   </si>
   <si>
     <t>LUCIA.MORENO@GMAIL.COM</t>
   </si>
   <si>
-    <t>DIEGO.SUAREZ@GMAIL.COM</t>
-  </si>
-  <si>
     <t>CARLOS</t>
   </si>
   <si>
@@ -280,6 +263,150 @@
   </si>
   <si>
     <t>GONZALEZ</t>
+  </si>
+  <si>
+    <t>PEDRO</t>
+  </si>
+  <si>
+    <t>LOPEZ</t>
+  </si>
+  <si>
+    <t>PEDRO.LOPEZ@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>ANA</t>
+  </si>
+  <si>
+    <t>GARCIA</t>
+  </si>
+  <si>
+    <t>MARTA</t>
+  </si>
+  <si>
+    <t>TORRES</t>
+  </si>
+  <si>
+    <t>MARTA.TORRES@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>LUIS</t>
+  </si>
+  <si>
+    <t>RAMIREZ</t>
+  </si>
+  <si>
+    <t>ANDREA</t>
+  </si>
+  <si>
+    <t>MENDOZA</t>
+  </si>
+  <si>
+    <t>ANDREA.MENDOZA@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>CASTRO</t>
+  </si>
+  <si>
+    <t>LAURA</t>
+  </si>
+  <si>
+    <t>SALAZAR</t>
+  </si>
+  <si>
+    <t>LAURA.SALAZAR@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>DANIEL</t>
+  </si>
+  <si>
+    <t>HERRERA</t>
+  </si>
+  <si>
+    <t>JULIA</t>
+  </si>
+  <si>
+    <t>REYES</t>
+  </si>
+  <si>
+    <t>JULIA.REYES@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>PABLO</t>
+  </si>
+  <si>
+    <t>RIVERA</t>
+  </si>
+  <si>
+    <t>ALBERTO</t>
+  </si>
+  <si>
+    <t>NAVARRO</t>
+  </si>
+  <si>
+    <t>ALBERTO.NAVARRO@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>VICTORIA</t>
+  </si>
+  <si>
+    <t>ROJAS</t>
+  </si>
+  <si>
+    <t>VICTORIA.ROJAS@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>RAUL</t>
+  </si>
+  <si>
+    <t>SOTO</t>
+  </si>
+  <si>
+    <t>RAUL.SOTO@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>ELENA</t>
+  </si>
+  <si>
+    <t>PEREIRA</t>
+  </si>
+  <si>
+    <t>ELENA.PEREIRA@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>VALENTINA</t>
+  </si>
+  <si>
+    <t>GOMEZ</t>
+  </si>
+  <si>
+    <t>MATEO</t>
+  </si>
+  <si>
+    <t>ALVAREZ</t>
+  </si>
+  <si>
+    <t>ISABEL</t>
+  </si>
+  <si>
+    <t>RAMOS</t>
+  </si>
+  <si>
+    <t>ORTEGA</t>
+  </si>
+  <si>
+    <t>FERRER</t>
+  </si>
+  <si>
+    <t>EMILIA</t>
+  </si>
+  <si>
+    <t>CASTILLO</t>
+  </si>
+  <si>
+    <t>tipo_doc</t>
+  </si>
+  <si>
+    <t>DNI</t>
   </si>
 </sst>
 </file>
@@ -353,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -385,12 +512,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="51">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -409,6 +539,46 @@
           <color theme="4"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF4472C4"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF4472C4"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF4472C4"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF4472C4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -734,7 +904,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1652CAA9-7C57-4CC6-AF28-FF59B7024886}" name="Tabla3" displayName="Tabla3" ref="A1:E4" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1652CAA9-7C57-4CC6-AF28-FF59B7024886}" name="Tabla3" displayName="Tabla3" ref="A1:E4" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" tableBorderDxfId="48">
   <autoFilter ref="A1:E4" xr:uid="{EC49B573-A6C0-438B-8D7D-6033A5C9240C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -743,18 +913,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AF1F70C4-EEAF-46BC-B521-48F7B8178DC1}" name="id" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{8D365490-8F6C-4CB3-A978-A767CF110BD2}" name="tipo" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{407BDEB2-50A9-4547-BE98-80B3548B87E2}" name="servicio" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{2E7B4E0A-59DD-4509-84CC-121416A1D0EA}" name="partida" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{4C6E8BCC-4CD2-453E-908C-0E6BD877430C}" name="destino" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{AF1F70C4-EEAF-46BC-B521-48F7B8178DC1}" name="id" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{8D365490-8F6C-4CB3-A978-A767CF110BD2}" name="tipo" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{407BDEB2-50A9-4547-BE98-80B3548B87E2}" name="servicio" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{2E7B4E0A-59DD-4509-84CC-121416A1D0EA}" name="partida" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{4C6E8BCC-4CD2-453E-908C-0E6BD877430C}" name="destino" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1342713E-B4EB-4B05-95AC-7413F77FCB87}" name="Tabla1" displayName="Tabla1" ref="A1:S4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1342713E-B4EB-4B05-95AC-7413F77FCB87}" name="Tabla1" displayName="Tabla1" ref="A1:S4" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="A1:S4" xr:uid="{9EAAADC5-9F46-43F9-86DA-9355898506F0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -777,33 +947,33 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{1B96264B-2CB3-47D7-B4C0-51870E444072}" name="Id" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{F471FA38-E69A-47DD-80E5-6DB2A13DA5F2}" name="tipo" dataDxfId="29"/>
-    <tableColumn id="27" xr3:uid="{593C92AB-FB00-425B-BAE4-125BCD359769}" name="n" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{2CB10096-B030-40AC-A185-5BAF05E5996A}" name="cab1 adulto" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{4BF48631-0A0C-4A8D-BDDC-A6363B600754}" name="cab1 ninho" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{782AF4A2-3991-40DA-87D7-CFBF36B6D3CF}" name="cab2 adulto" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{2D21EED6-3A13-4F76-B9EB-3D0CEDBA098A}" name="cab2 ninho" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{B3826654-211E-4333-8145-ED5B6A0713B3}" name="cab3 adulto" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{66740B94-F52D-4E67-9DE4-A6F7D5C1D86A}" name="cab3 ninho" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{ABC75B57-996C-499F-A86A-BEF43DA1822A}" name="cab4 adulto" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{742E54BC-8B8A-46CA-86E8-E57426D99AA0}" name="cab4 ninho" dataDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{0C3C72A8-0EFF-4257-89CF-DA314D58045D}" name="cab5 adulto" dataDxfId="19"/>
-    <tableColumn id="17" xr3:uid="{1B1E8A8C-8FE2-4FB4-A0B3-D6B67CCE0051}" name="cab5 ninho" dataDxfId="18"/>
-    <tableColumn id="18" xr3:uid="{B3CE59D7-3C6F-493F-B16E-90E99B4687E8}" name="cab6 adulto" dataDxfId="17"/>
-    <tableColumn id="20" xr3:uid="{883376CA-564F-46C6-A8AA-1ABBCFB17391}" name="cab6 ninho" dataDxfId="16"/>
-    <tableColumn id="21" xr3:uid="{A554B50B-B826-42AE-BF9F-6322C26F7556}" name="cab7 adulto" dataDxfId="15"/>
-    <tableColumn id="23" xr3:uid="{E47090D1-C062-483F-8F35-AB1D2E620891}" name="cab7 ninho" dataDxfId="14"/>
-    <tableColumn id="24" xr3:uid="{67CFF31E-6EEB-436D-966A-F6924BE14906}" name="cab8 adulto" dataDxfId="13"/>
-    <tableColumn id="26" xr3:uid="{62CF0A50-024F-419D-A148-FE2CD3007DED}" name="cab8 ninho" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{1B96264B-2CB3-47D7-B4C0-51870E444072}" name="Id" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{F471FA38-E69A-47DD-80E5-6DB2A13DA5F2}" name="tipo" dataDxfId="38"/>
+    <tableColumn id="27" xr3:uid="{593C92AB-FB00-425B-BAE4-125BCD359769}" name="n" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{2CB10096-B030-40AC-A185-5BAF05E5996A}" name="cab1 adulto" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{4BF48631-0A0C-4A8D-BDDC-A6363B600754}" name="cab1 ninho" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{782AF4A2-3991-40DA-87D7-CFBF36B6D3CF}" name="cab2 adulto" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{2D21EED6-3A13-4F76-B9EB-3D0CEDBA098A}" name="cab2 ninho" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{B3826654-211E-4333-8145-ED5B6A0713B3}" name="cab3 adulto" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{66740B94-F52D-4E67-9DE4-A6F7D5C1D86A}" name="cab3 ninho" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{ABC75B57-996C-499F-A86A-BEF43DA1822A}" name="cab4 adulto" dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{742E54BC-8B8A-46CA-86E8-E57426D99AA0}" name="cab4 ninho" dataDxfId="29"/>
+    <tableColumn id="15" xr3:uid="{0C3C72A8-0EFF-4257-89CF-DA314D58045D}" name="cab5 adulto" dataDxfId="28"/>
+    <tableColumn id="17" xr3:uid="{1B1E8A8C-8FE2-4FB4-A0B3-D6B67CCE0051}" name="cab5 ninho" dataDxfId="27"/>
+    <tableColumn id="18" xr3:uid="{B3CE59D7-3C6F-493F-B16E-90E99B4687E8}" name="cab6 adulto" dataDxfId="26"/>
+    <tableColumn id="20" xr3:uid="{883376CA-564F-46C6-A8AA-1ABBCFB17391}" name="cab6 ninho" dataDxfId="25"/>
+    <tableColumn id="21" xr3:uid="{A554B50B-B826-42AE-BF9F-6322C26F7556}" name="cab7 adulto" dataDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{E47090D1-C062-483F-8F35-AB1D2E620891}" name="cab7 ninho" dataDxfId="23"/>
+    <tableColumn id="24" xr3:uid="{67CFF31E-6EEB-436D-966A-F6924BE14906}" name="cab8 adulto" dataDxfId="22"/>
+    <tableColumn id="26" xr3:uid="{62CF0A50-024F-419D-A148-FE2CD3007DED}" name="cab8 ninho" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87305A22-35F9-42EC-9298-4EBF5F16E71E}" name="Tabla4" displayName="Tabla4" ref="A1:J10" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A1:J10" xr:uid="{A59B09B4-BE40-4769-A458-C2BBB98E1FD2}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{87305A22-35F9-42EC-9298-4EBF5F16E71E}" name="Tabla4" displayName="Tabla4" ref="A1:J16" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="A1:J16" xr:uid="{A59B09B4-BE40-4769-A458-C2BBB98E1FD2}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -816,15 +986,15 @@
     <filterColumn colId="9" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{A67B8055-A31F-4E61-B923-53E93F83D94D}" name="id" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{E4C9E876-2CE6-46DD-ABF6-BD84C1ABADE0}" name="tipo" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{A67B8055-A31F-4E61-B923-53E93F83D94D}" name="id" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{4EFD328A-F656-4EB3-BAF8-BBFE9DA54446}" name="nombre"/>
     <tableColumn id="3" xr3:uid="{B64115F5-DB6E-4390-9D72-B28B899FBE63}" name="apellido"/>
-    <tableColumn id="4" xr3:uid="{371A0582-D500-48FA-9125-FE8C3A19B89D}" name="genero" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{553FB7E9-1C69-4B90-AF93-03D6DB9D2E9B}" name="pais" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{D44FC6FC-48E1-4D14-AA44-6EAC0ED03876}" name="dni" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{14698F99-1A4C-4D41-AD0C-1EE9DD2E71C6}" name="cumpleanhos" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{D44FF9C0-E498-4360-B1D1-2F753CE8B9E1}" name="telefono" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{371A0582-D500-48FA-9125-FE8C3A19B89D}" name="genero" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{553FB7E9-1C69-4B90-AF93-03D6DB9D2E9B}" name="pais" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{FFC7D024-C5BB-4047-8446-51816114B34F}" name="tipo_doc" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{D44FC6FC-48E1-4D14-AA44-6EAC0ED03876}" name="dni" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{14698F99-1A4C-4D41-AD0C-1EE9DD2E71C6}" name="cumpleanhos" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{D44FF9C0-E498-4360-B1D1-2F753CE8B9E1}" name="telefono" dataDxfId="11"/>
     <tableColumn id="9" xr3:uid="{68E432A6-4D1E-4442-8D04-4B3C3DD39AD1}" name="correo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -832,6 +1002,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{67FB4A38-0531-4C69-BB40-A037250FAD4B}" name="Tabla47" displayName="Tabla47" ref="A1:H16" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="A1:H16" xr:uid="{A59B09B4-BE40-4769-A458-C2BBB98E1FD2}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F059D60E-8F1A-4D33-AA38-93D3067C1431}" name="id" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{2C96B92C-9750-4B2B-8835-58C5A3EC7452}" name="nombre"/>
+    <tableColumn id="3" xr3:uid="{2859A837-8EF5-4B3C-A003-D2F7C05B1321}" name="apellido"/>
+    <tableColumn id="4" xr3:uid="{BB5E12A6-6EB3-4CFB-BD01-4B73952DBAEA}" name="genero" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{98A2E86B-41E7-49F2-A05C-9A19D9CF07BD}" name="pais" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{511E5AAD-DBCB-4010-9835-C1AA2C739DD6}" name="tipo_doc" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{9678B705-E6DB-4D1B-97E9-D7D79E5931FC}" name="dni" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{8404C0CE-1696-46BC-8763-153E8B479FCE}" name="cumpleanhos" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{541625AD-5C97-4AD0-BBB7-D671FD0CF7AA}" name="Tabla2" displayName="Tabla2" ref="A1:B5" totalsRowShown="0" tableBorderDxfId="1">
   <autoFilter ref="A1:B5" xr:uid="{5AF637C0-FB21-4C41-BD79-56E1E1BC8907}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -1145,7 +1341,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1433,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="S4" sqref="A1:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,52 +1451,52 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>38</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>39</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>40</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>41</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>42</v>
       </c>
       <c r="N1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>43</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S1" s="8" t="s">
         <v>44</v>
@@ -1311,7 +1507,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3">
         <v>2</v>
@@ -1497,18 +1693,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA7E65F2-5786-4038-91E1-AB94B5AD9FAC}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="4"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="4" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="4"/>
     <col min="7" max="9" width="15.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="30.7109375" customWidth="1"/>
   </cols>
@@ -1517,20 +1713,20 @@
       <c r="A1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E1" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>12</v>
@@ -1549,20 +1745,20 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>58</v>
+      <c r="B2" t="s">
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
         <v>16</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>125</v>
       </c>
       <c r="G2" s="4">
         <v>10000001</v>
@@ -1581,20 +1777,20 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>58</v>
+      <c r="B3" t="s">
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
         <v>36</v>
       </c>
+      <c r="D3" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>125</v>
       </c>
       <c r="G3" s="4">
         <v>10000002</v>
@@ -1613,246 +1809,876 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="4">
+        <v>10000004</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4">
-        <v>10000003</v>
-      </c>
-      <c r="H4" s="6">
-        <v>39617</v>
-      </c>
       <c r="I4" s="4">
-        <v>999888779</v>
+        <v>999888780</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>58</v>
+      <c r="B5" t="s">
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
+        <v>76</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="G5" s="4">
-        <v>10000004</v>
+        <v>10000005</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="4">
+        <v>999888781</v>
+      </c>
+      <c r="J5" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="I5" s="4">
-        <v>999888780</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>58</v>
+      <c r="B6" t="s">
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>82</v>
+        <v>69</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="G6" s="4">
-        <v>10000005</v>
-      </c>
-      <c r="H6" s="4" t="s">
+        <v>10000007</v>
+      </c>
+      <c r="H6" s="6">
+        <v>35861</v>
+      </c>
+      <c r="I6" s="4">
+        <v>999888783</v>
+      </c>
+      <c r="J6" s="12" t="s">
         <v>64</v>
-      </c>
-      <c r="I6" s="4">
-        <v>999888781</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>59</v>
+      <c r="B7" t="s">
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>81</v>
+        <v>70</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="G7" s="4">
-        <v>10000006</v>
-      </c>
-      <c r="H7" s="6">
-        <v>40037</v>
+        <v>10000008</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="I7" s="4">
-        <v>999888782</v>
+        <v>999888784</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>58</v>
+      <c r="B8" t="s">
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="G8" s="4">
-        <v>10000007</v>
+        <v>10000010</v>
       </c>
       <c r="H8" s="6">
-        <v>35861</v>
+        <v>32084</v>
       </c>
       <c r="I8" s="4">
-        <v>999888783</v>
+        <v>999888786</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>58</v>
+      <c r="B9" t="s">
+        <v>83</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="G9" s="4">
-        <v>10000008</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>65</v>
+        <v>10000012</v>
+      </c>
+      <c r="H9" s="6">
+        <v>35045</v>
       </c>
       <c r="I9" s="4">
-        <v>999888784</v>
+        <v>999888788</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>59</v>
+      <c r="B10" t="s">
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" t="s">
-        <v>77</v>
+        <v>89</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="4">
+        <v>10000014</v>
+      </c>
+      <c r="H10" s="6">
+        <v>34014</v>
+      </c>
+      <c r="I10" s="4">
+        <v>999888790</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="4">
+        <v>10000016</v>
+      </c>
+      <c r="H11" s="6">
+        <v>32964</v>
+      </c>
+      <c r="I11" s="4">
+        <v>999888792</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="4">
+        <v>10000018</v>
+      </c>
+      <c r="H12" s="6">
+        <v>32515</v>
+      </c>
+      <c r="I12" s="4">
+        <v>999888794</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="4">
-        <v>10000009</v>
-      </c>
-      <c r="H10" s="6">
-        <v>40180</v>
-      </c>
-      <c r="I10" s="4">
-        <v>999888785</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>71</v>
+      <c r="E13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="4">
+        <v>10000020</v>
+      </c>
+      <c r="H13" s="6">
+        <v>32188</v>
+      </c>
+      <c r="I13" s="4">
+        <v>999888796</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="4">
+        <v>10000021</v>
+      </c>
+      <c r="H14" s="6">
+        <v>34647</v>
+      </c>
+      <c r="I14" s="4">
+        <v>999888797</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="4">
+        <v>10000022</v>
+      </c>
+      <c r="H15" s="6">
+        <v>31641</v>
+      </c>
+      <c r="I15" s="4">
+        <v>999888798</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="4">
+        <v>10000023</v>
+      </c>
+      <c r="H16" s="6">
+        <v>33370</v>
+      </c>
+      <c r="I16" s="4">
+        <v>999888799</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{EDBE7E2E-DF90-4605-BB0E-E8CF6B41AC41}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{B2FCA654-2C91-46BB-9DAD-1788CF7E4EAD}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{E97F2C90-A4BB-4694-9B1B-52934912DD2B}"/>
-    <hyperlink ref="J5" r:id="rId4" xr:uid="{DF9663D3-B01E-46EF-A09A-4DBE4CECECE5}"/>
-    <hyperlink ref="J6" r:id="rId5" xr:uid="{20E7BBE3-8014-4468-8C52-DEC6E4C6479A}"/>
-    <hyperlink ref="J7" r:id="rId6" xr:uid="{A797241E-92CF-4A97-AD88-E955311FBF43}"/>
-    <hyperlink ref="J8" r:id="rId7" xr:uid="{35CE8E0C-2660-4268-A92B-584BF595697F}"/>
-    <hyperlink ref="J9" r:id="rId8" xr:uid="{81B60F69-6326-42B7-85C0-B33B153BB8B3}"/>
-    <hyperlink ref="J10" r:id="rId9" xr:uid="{EEB17FD2-DDD6-4B99-A5ED-6EB9B1D56F90}"/>
+    <hyperlink ref="J13" r:id="rId1" xr:uid="{86FE29EA-F8B3-47CF-B763-F1D46B245B3C}"/>
+    <hyperlink ref="J14" r:id="rId2" xr:uid="{82B8CDDD-679A-453B-9B58-9967767EEC61}"/>
+    <hyperlink ref="J15" r:id="rId3" xr:uid="{A40106A8-F72E-41CC-AAE6-A8DCFC4A4AE8}"/>
+    <hyperlink ref="J16" r:id="rId4" xr:uid="{05776B7A-AC45-4BFC-A74F-A9FAE32C1610}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9A648F-C257-45DC-A7DB-C343F007425A}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="4" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="4"/>
+    <col min="7" max="8" width="15.7109375" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G2" s="4">
+        <v>10000003</v>
+      </c>
+      <c r="H2" s="6">
+        <v>39617</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="4">
+        <v>10000006</v>
+      </c>
+      <c r="H3" s="6">
+        <v>40037</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="4">
+        <v>10000009</v>
+      </c>
+      <c r="H4" s="6">
+        <v>40180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="4">
+        <v>10000011</v>
+      </c>
+      <c r="H5" s="6">
+        <v>38494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="4">
+        <v>10000013</v>
+      </c>
+      <c r="H6" s="6">
+        <v>40754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="4">
+        <v>10000015</v>
+      </c>
+      <c r="H7" s="6">
+        <v>39330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G8" s="4">
+        <v>10000017</v>
+      </c>
+      <c r="H8" s="6">
+        <v>39009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="4">
+        <v>10000019</v>
+      </c>
+      <c r="H9" s="6">
+        <v>39622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="4">
+        <v>10000024</v>
+      </c>
+      <c r="H10" s="6">
+        <v>39880</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="4">
+        <v>10000025</v>
+      </c>
+      <c r="H11" s="6">
+        <v>40443</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="4">
+        <v>10000026</v>
+      </c>
+      <c r="H12" s="6">
+        <v>39268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="4">
+        <v>10000027</v>
+      </c>
+      <c r="H13" s="6">
+        <v>39458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G14" s="4">
+        <v>10000028</v>
+      </c>
+      <c r="H14" s="6">
+        <v>40902</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" s="4">
+        <v>10000029</v>
+      </c>
+      <c r="H15" s="6">
+        <v>38821</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G16" s="4">
+        <v>10000030</v>
+      </c>
+      <c r="H16" s="6">
+        <v>41187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819BDDB9-123C-42C7-8772-2B03ABCF962E}">
   <dimension ref="A1:D10"/>
   <sheetViews>

</xml_diff>